<commit_message>
[internal] add: 8 fairies
</commit_message>
<xml_diff>
--- a/FairyList.xlsx
+++ b/FairyList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\GitHub\MirageFairy2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58ED18A6-DEDD-4ED0-84D3-D901C7B723E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B4653F-029C-4BB5-8F3A-4A17C5F072CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{50F21D03-37BB-40FB-A570-1AD8030E22E9}"/>
+    <workbookView xWindow="5400" yWindow="1950" windowWidth="17970" windowHeight="13230" xr2:uid="{50F21D03-37BB-40FB-A570-1AD8030E22E9}"/>
   </bookViews>
   <sheets>
     <sheet name="妖精リスト" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="1092">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -4636,53 +4636,6 @@
     <t>0xFFECB8, 0xFFFF0B, 0xDC7613, 0xFFEE97</t>
   </si>
   <si>
-    <t>null140</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>null141</t>
-  </si>
-  <si>
-    <t>null142</t>
-  </si>
-  <si>
-    <t>null143</t>
-  </si>
-  <si>
-    <t>null144</t>
-  </si>
-  <si>
-    <t>null145</t>
-  </si>
-  <si>
-    <t>null146</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000000</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000001</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000002</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000003</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000004</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000005</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000006</t>
-  </si>
-  <si>
-    <t>0xFF00FF, 0xFF00FF, 0x000000, 0x000007</t>
-  </si>
-  <si>
     <t>紅玉精</t>
     <rPh sb="0" eb="2">
       <t>コウギョク</t>
@@ -4693,16 +4646,172 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>gravity</t>
+  </si>
+  <si>
+    <t>重力精</t>
+    <rPh sb="0" eb="2">
+      <t>ジュウリョク</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>岩盤精</t>
+  </si>
+  <si>
+    <t>本精</t>
+  </si>
+  <si>
+    <t>釦精</t>
+  </si>
+  <si>
+    <t>button</t>
+  </si>
+  <si>
+    <t>蝙蝠精</t>
+    <rPh sb="0" eb="2">
+      <t>コウモリ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bat</t>
+  </si>
+  <si>
+    <t>消滅呪精</t>
+    <rPh sb="3" eb="4">
+      <t>セイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>curse_of_vanishing</t>
+  </si>
+  <si>
+    <t>cooked_cod</t>
+  </si>
+  <si>
+    <t>焼鱈精</t>
+    <rPh sb="0" eb="1">
+      <t>ヤ</t>
+    </rPh>
+    <rPh sb="1" eb="2">
+      <t>タラ</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>セイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>peony</t>
+  </si>
+  <si>
+    <t>牡丹精</t>
+    <rPh sb="0" eb="2">
+      <t>ボタン</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>セイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ルービャ</t>
+  </si>
+  <si>
     <t>Rubia</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>ruby</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>ルービャ</t>
-    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>グラヴィーチャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ベドロッキャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ボーキャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブットーニャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>バーチャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ツルセオフェヴァニシンギャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ツォーケーデツォージャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Gravitia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bedrockia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Bookia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Buttonia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Batia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Curse Ofe Vanishingia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Cookede Codia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ペオーニャ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Peonia</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x7C7C7C, 0xB4B4B4, 0x484848, 0x040404</t>
+  </si>
+  <si>
+    <t>0x4C3E30, 0x5B482B, 0x2C2014, 0x221F1D</t>
+  </si>
+  <si>
+    <t>0x63D700, 0xEDD6F7, 0xEDD6F7, 0xDEA5F7</t>
+  </si>
+  <si>
+    <t>0xD6D6D6, 0x654B17, 0x654B17, 0x000000</t>
+  </si>
+  <si>
+    <t>0xC4B1B4, 0xC4B1B4, 0xC4B1B4, 0x6B9F93</t>
+  </si>
+  <si>
+    <t>0xD0C2FF, 0xFF003B, 0x370000, 0xE2BBFF</t>
+  </si>
+  <si>
+    <t>0xFFFFFF, 0xBC9862, 0xBC9862, 0xD40102</t>
+  </si>
+  <si>
+    <t>0xC2A7F2, 0x3600FF, 0x2A00B1, 0x110047</t>
   </si>
 </sst>
 </file>
@@ -4729,7 +4838,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4778,6 +4887,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -4793,7 +4908,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4848,11 +4963,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="255" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="65">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.249977111117893"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -5252,35 +5399,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.249977111117893"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -5477,77 +5595,77 @@
     <tableColumn id="7" xr3:uid="{B7A1B9A3-3658-4251-9488-C7EB28DDA828}" name="基礎Wind" dataDxfId="48"/>
     <tableColumn id="8" xr3:uid="{53D9BDAB-CC6B-4E70-8605-30718A287EC4}" name="基礎Gaia" dataDxfId="47"/>
     <tableColumn id="9" xr3:uid="{EB888AF3-8815-48CE-A95E-C5931929A1AC}" name="基礎Aqua" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{68F80D1D-DFED-4D2F-92EF-7D17590D4A36}" name="基礎Dark" dataDxfId="45"/>
-    <tableColumn id="45" xr3:uid="{0A19614E-0FAE-4CB9-94EF-E0B3FBBD091F}" name="特殊倍率" dataDxfId="44"/>
-    <tableColumn id="13" xr3:uid="{D846AE64-655F-4052-B5F1-3F4B9699D0FA}" name="レア度倍率" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{68F80D1D-DFED-4D2F-92EF-7D17590D4A36}" name="基礎Dark" dataDxfId="2"/>
+    <tableColumn id="45" xr3:uid="{0A19614E-0FAE-4CB9-94EF-E0B3FBBD091F}" name="特殊倍率" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{D846AE64-655F-4052-B5F1-3F4B9699D0FA}" name="レア度倍率" dataDxfId="1">
       <calculatedColumnFormula>2^((テーブル1[[#This Row],[レア]]-1)/4)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{833C82E7-E230-4A58-9D49-6C1CDD4BBDAD}" name="分散度倍率" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{833C82E7-E230-4A58-9D49-6C1CDD4BBDAD}" name="分散度倍率" dataDxfId="45">
       <calculatedColumnFormula>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M2:R2)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{434606B6-C04F-47DC-9277-0797C7617151}" name="効率" dataDxfId="41">
+    <tableColumn id="22" xr3:uid="{434606B6-C04F-47DC-9277-0797C7617151}" name="効率" dataDxfId="44">
       <calculatedColumnFormula>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{B031CBD1-7BDB-4552-BC58-A8FCCA491403}" name="合計値" dataDxfId="40">
+    <tableColumn id="15" xr3:uid="{B031CBD1-7BDB-4552-BC58-A8FCCA491403}" name="合計値" dataDxfId="43">
       <calculatedColumnFormula>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{FCD4377E-4837-4BD9-8716-12CB589EDF74}" name="Shine" dataDxfId="39">
+    <tableColumn id="16" xr3:uid="{FCD4377E-4837-4BD9-8716-12CB589EDF74}" name="Shine" dataDxfId="42">
       <calculatedColumnFormula>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{192E8193-ED35-4778-87AC-0C1CF273DBF9}" name="Fire" dataDxfId="38">
+    <tableColumn id="17" xr3:uid="{192E8193-ED35-4778-87AC-0C1CF273DBF9}" name="Fire" dataDxfId="41">
       <calculatedColumnFormula>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{FDD6FC8F-4CBF-4964-A0D2-682E72230537}" name="Wind" dataDxfId="37">
+    <tableColumn id="18" xr3:uid="{FDD6FC8F-4CBF-4964-A0D2-682E72230537}" name="Wind" dataDxfId="40">
       <calculatedColumnFormula>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{DE083808-871E-4527-B7C9-FF57A44BDF23}" name="Gaia" dataDxfId="36">
+    <tableColumn id="19" xr3:uid="{DE083808-871E-4527-B7C9-FF57A44BDF23}" name="Gaia" dataDxfId="39">
       <calculatedColumnFormula>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{EEDF52F6-D7AB-4A1B-B203-856E8CD45BA9}" name="Aqua" dataDxfId="35">
+    <tableColumn id="20" xr3:uid="{EEDF52F6-D7AB-4A1B-B203-856E8CD45BA9}" name="Aqua" dataDxfId="38">
       <calculatedColumnFormula>テーブル1[[#This Row],[基礎Aqua]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{61A17369-9D3E-4EE3-B6BB-316F47062244}" name="Dark" dataDxfId="34">
+    <tableColumn id="21" xr3:uid="{61A17369-9D3E-4EE3-B6BB-316F47062244}" name="Dark" dataDxfId="37">
       <calculatedColumnFormula>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{FF31EB97-6C72-4B4F-9C7D-7FE5546BDC56}" name="攻撃" dataDxfId="33"/>
-    <tableColumn id="44" xr3:uid="{D91E944B-F524-4F9B-9D06-B8EE217F8C86}" name="加工" dataDxfId="32"/>
-    <tableColumn id="48" xr3:uid="{FDAEB361-38D6-4EFA-B314-79F5DF42167E}" name="収穫" dataDxfId="31"/>
-    <tableColumn id="46" xr3:uid="{ECCD46C1-F4EB-408C-AEB7-098E1A6BA65B}" name="発光" dataDxfId="30"/>
-    <tableColumn id="47" xr3:uid="{E006FC6A-6503-4BBD-94D8-3FBB62985153}" name="火炎" dataDxfId="29"/>
-    <tableColumn id="49" xr3:uid="{2BF29954-473B-4B0C-9781-028B561200CB}" name="流水" dataDxfId="28"/>
-    <tableColumn id="24" xr3:uid="{E078FC75-CC53-492A-A97D-107EA20B4296}" name="結晶" dataDxfId="27"/>
-    <tableColumn id="25" xr3:uid="{3CFDC570-BDAB-4914-ABC3-2C36BC441EFF}" name="音波" dataDxfId="26"/>
-    <tableColumn id="27" xr3:uid="{57B5D258-645E-405C-8646-A5BA9977E94A}" name="空間" dataDxfId="25"/>
-    <tableColumn id="28" xr3:uid="{FC7CB677-4A50-4B6E-A9B9-30E79C62F98D}" name="縮地" dataDxfId="24"/>
-    <tableColumn id="29" xr3:uid="{0A208B09-58DF-41DC-8C05-5263F315034B}" name="射出" dataDxfId="23"/>
-    <tableColumn id="31" xr3:uid="{B7C69519-DEF6-4AE2-A3F5-853F5A3D600F}" name="破壊" dataDxfId="22"/>
-    <tableColumn id="32" xr3:uid="{EF23F12F-E8B4-4880-9CA7-0217FC0413E6}" name="化学" dataDxfId="21"/>
-    <tableColumn id="33" xr3:uid="{D40F96E4-B2C9-4D5D-AB4C-D11CBE93B14C}" name="切断" dataDxfId="20"/>
-    <tableColumn id="42" xr3:uid="{DF3E8FB8-984D-4C55-A75B-2EEC0C39F73E}" name="生命" dataDxfId="19"/>
-    <tableColumn id="50" xr3:uid="{EB8957B0-BD4F-49BA-B5B3-34135A2A5AB9}" name="知識" dataDxfId="18"/>
-    <tableColumn id="51" xr3:uid="{74B52C90-EB55-4AE9-A15D-8796B683F98B}" name="熱量" dataDxfId="17"/>
-    <tableColumn id="52" xr3:uid="{1062E5CB-E53F-44AF-BD18-760F21295B80}" name="服従" dataDxfId="16"/>
-    <tableColumn id="54" xr3:uid="{16EB0B8E-63F6-4CC7-8AD5-1873DC69BE97}" name="聖夜" dataDxfId="15"/>
-    <tableColumn id="55" xr3:uid="{F01B7328-12B2-480D-8ACF-8B313E56A8FF}" name="氷結" dataDxfId="14"/>
-    <tableColumn id="56" xr3:uid="{2CB25BA5-84E8-4DA2-999F-21D7DB627A47}" name="雷電" dataDxfId="13"/>
-    <tableColumn id="36" xr3:uid="{28ACBEB8-30BE-4E7B-A2F5-111830028C94}" name="浮揚" dataDxfId="12"/>
-    <tableColumn id="41" xr3:uid="{6678BFE5-51F7-41C1-8093-03F1ED04C498}" name="感覚" dataDxfId="11"/>
-    <tableColumn id="53" xr3:uid="{0700EC90-BD06-48B4-A682-B65581165E4E}" name="超能力合計" dataDxfId="10">
+    <tableColumn id="40" xr3:uid="{FF31EB97-6C72-4B4F-9C7D-7FE5546BDC56}" name="攻撃" dataDxfId="36"/>
+    <tableColumn id="44" xr3:uid="{D91E944B-F524-4F9B-9D06-B8EE217F8C86}" name="加工" dataDxfId="35"/>
+    <tableColumn id="48" xr3:uid="{FDAEB361-38D6-4EFA-B314-79F5DF42167E}" name="収穫" dataDxfId="34"/>
+    <tableColumn id="46" xr3:uid="{ECCD46C1-F4EB-408C-AEB7-098E1A6BA65B}" name="発光" dataDxfId="33"/>
+    <tableColumn id="47" xr3:uid="{E006FC6A-6503-4BBD-94D8-3FBB62985153}" name="火炎" dataDxfId="32"/>
+    <tableColumn id="49" xr3:uid="{2BF29954-473B-4B0C-9781-028B561200CB}" name="流水" dataDxfId="31"/>
+    <tableColumn id="24" xr3:uid="{E078FC75-CC53-492A-A97D-107EA20B4296}" name="結晶" dataDxfId="30"/>
+    <tableColumn id="25" xr3:uid="{3CFDC570-BDAB-4914-ABC3-2C36BC441EFF}" name="音波" dataDxfId="29"/>
+    <tableColumn id="27" xr3:uid="{57B5D258-645E-405C-8646-A5BA9977E94A}" name="空間" dataDxfId="28"/>
+    <tableColumn id="28" xr3:uid="{FC7CB677-4A50-4B6E-A9B9-30E79C62F98D}" name="縮地" dataDxfId="27"/>
+    <tableColumn id="29" xr3:uid="{0A208B09-58DF-41DC-8C05-5263F315034B}" name="射出" dataDxfId="26"/>
+    <tableColumn id="31" xr3:uid="{B7C69519-DEF6-4AE2-A3F5-853F5A3D600F}" name="破壊" dataDxfId="25"/>
+    <tableColumn id="32" xr3:uid="{EF23F12F-E8B4-4880-9CA7-0217FC0413E6}" name="化学" dataDxfId="24"/>
+    <tableColumn id="33" xr3:uid="{D40F96E4-B2C9-4D5D-AB4C-D11CBE93B14C}" name="切断" dataDxfId="23"/>
+    <tableColumn id="42" xr3:uid="{DF3E8FB8-984D-4C55-A75B-2EEC0C39F73E}" name="生命" dataDxfId="22"/>
+    <tableColumn id="50" xr3:uid="{EB8957B0-BD4F-49BA-B5B3-34135A2A5AB9}" name="知識" dataDxfId="21"/>
+    <tableColumn id="51" xr3:uid="{74B52C90-EB55-4AE9-A15D-8796B683F98B}" name="熱量" dataDxfId="20"/>
+    <tableColumn id="52" xr3:uid="{1062E5CB-E53F-44AF-BD18-760F21295B80}" name="服従" dataDxfId="19"/>
+    <tableColumn id="54" xr3:uid="{16EB0B8E-63F6-4CC7-8AD5-1873DC69BE97}" name="聖夜" dataDxfId="18"/>
+    <tableColumn id="55" xr3:uid="{F01B7328-12B2-480D-8ACF-8B313E56A8FF}" name="氷結" dataDxfId="17"/>
+    <tableColumn id="56" xr3:uid="{2CB25BA5-84E8-4DA2-999F-21D7DB627A47}" name="雷電" dataDxfId="16"/>
+    <tableColumn id="36" xr3:uid="{28ACBEB8-30BE-4E7B-A2F5-111830028C94}" name="浮揚" dataDxfId="15"/>
+    <tableColumn id="41" xr3:uid="{6678BFE5-51F7-41C1-8093-03F1ED04C498}" name="感覚" dataDxfId="14"/>
+    <tableColumn id="53" xr3:uid="{0700EC90-BD06-48B4-A682-B65581165E4E}" name="超能力合計" dataDxfId="13">
       <calculatedColumnFormula>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="58" xr3:uid="{D7667722-AA3E-47DA-BB91-4A2DAE063B4B}" name="Camel Case" dataDxfId="9">
+    <tableColumn id="58" xr3:uid="{D7667722-AA3E-47DA-BB91-4A2DAE063B4B}" name="Camel Case" dataDxfId="12">
       <calculatedColumnFormula>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{163385B1-C9C9-410C-ABD5-0FB9C9D39FBB}" name="Code Kotlin" dataDxfId="8">
+    <tableColumn id="35" xr3:uid="{163385B1-C9C9-410C-ABD5-0FB9C9D39FBB}" name="Code Kotlin" dataDxfId="11">
       <calculatedColumnFormula array="1">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{4F31450C-EC23-4854-A316-C804DD0EAC46}" name="Code英名" dataDxfId="7">
+    <tableColumn id="37" xr3:uid="{4F31450C-EC23-4854-A316-C804DD0EAC46}" name="Code英名" dataDxfId="10">
       <calculatedColumnFormula>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{87187A24-E0A4-40E3-9C23-0138D3146A81}" name="Code和名" dataDxfId="6">
+    <tableColumn id="38" xr3:uid="{87187A24-E0A4-40E3-9C23-0138D3146A81}" name="Code和名" dataDxfId="9">
       <calculatedColumnFormula>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{9C44ECA8-EED1-4BD0-8581-195BA4A1A6EE}" name="フリー関数" dataDxfId="5">
+    <tableColumn id="43" xr3:uid="{9C44ECA8-EED1-4BD0-8581-195BA4A1A6EE}" name="フリー関数" dataDxfId="8">
       <calculatedColumnFormula>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5556,14 +5674,14 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C62C1D26-960A-48CC-8F29-5C012BAB8C70}" name="テーブル2" displayName="テーブル2" ref="A1:B69" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C62C1D26-960A-48CC-8F29-5C012BAB8C70}" name="テーブル2" displayName="テーブル2" ref="A1:B69" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="A1:B69" xr:uid="{FEC50A1C-B428-4AD7-9BA5-4DA035F73E38}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A69">
     <sortCondition ref="A1:A69"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{7E14A5CD-7281-42C1-93CF-8BD7C74666AC}" name="name" dataDxfId="2"/>
-    <tableColumn id="15" xr3:uid="{60E9BA99-755B-467A-9053-1708ABE43FE6}" name="列1" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{7E14A5CD-7281-42C1-93CF-8BD7C74666AC}" name="name" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{60E9BA99-755B-467A-9053-1708ABE43FE6}" name="列1" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5587,7 +5705,7 @@
     <tableColumn id="8" xr3:uid="{C37B4482-84AD-481D-914C-03A51BD0F6FA}" name="列8">
       <calculatedColumnFormula>F2*G2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{B2463834-F42F-4CD7-BEC9-B542CC83738A}" name="列9" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{B2463834-F42F-4CD7-BEC9-B542CC83738A}" name="列9" dataDxfId="3">
       <calculatedColumnFormula>"ItemFairyCrystal.drops.add(new Drop(ModuleFairy.FairyTypes."&amp;C2&amp;"[0].createItemStack(), "&amp;H2&amp;"));"</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5861,10 +5979,10 @@
   <dimension ref="A1:BF157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="6" ySplit="1" topLeftCell="AB140" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="1" topLeftCell="AN134" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BC143" sqref="BC143"/>
+      <selection pane="bottomRight" activeCell="BC2" sqref="BC2:BC151"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6113,7 +6231,7 @@
       <c r="R2" s="7">
         <v>10</v>
       </c>
-      <c r="S2" s="5">
+      <c r="S2" s="18">
         <v>1</v>
       </c>
       <c r="T2" s="5">
@@ -6269,7 +6387,7 @@
       <c r="R3" s="7">
         <v>10</v>
       </c>
-      <c r="S3" s="5">
+      <c r="S3" s="18">
         <v>1</v>
       </c>
       <c r="T3" s="5">
@@ -6429,7 +6547,7 @@
       <c r="R4" s="7">
         <v>10</v>
       </c>
-      <c r="S4" s="5">
+      <c r="S4" s="18">
         <v>1</v>
       </c>
       <c r="T4" s="5">
@@ -6597,7 +6715,7 @@
       <c r="R5" s="7">
         <v>60</v>
       </c>
-      <c r="S5" s="5">
+      <c r="S5" s="18">
         <v>1</v>
       </c>
       <c r="T5" s="5">
@@ -6751,7 +6869,7 @@
       <c r="R6" s="7">
         <v>10</v>
       </c>
-      <c r="S6" s="5">
+      <c r="S6" s="18">
         <v>1</v>
       </c>
       <c r="T6" s="5">
@@ -6903,7 +7021,7 @@
       <c r="R7" s="7">
         <v>10</v>
       </c>
-      <c r="S7" s="5">
+      <c r="S7" s="18">
         <v>1</v>
       </c>
       <c r="T7" s="5">
@@ -7057,7 +7175,7 @@
       <c r="R8" s="7">
         <v>4</v>
       </c>
-      <c r="S8" s="5">
+      <c r="S8" s="18">
         <v>1</v>
       </c>
       <c r="T8" s="5">
@@ -7219,7 +7337,7 @@
         <v>23</v>
       </c>
       <c r="R9" s="7"/>
-      <c r="S9" s="5">
+      <c r="S9" s="18">
         <v>1</v>
       </c>
       <c r="T9" s="5">
@@ -7383,7 +7501,7 @@
       <c r="R10" s="7">
         <v>6</v>
       </c>
-      <c r="S10" s="5">
+      <c r="S10" s="18">
         <v>1</v>
       </c>
       <c r="T10" s="5">
@@ -7549,7 +7667,7 @@
       <c r="R11" s="7">
         <v>1</v>
       </c>
-      <c r="S11" s="5">
+      <c r="S11" s="18">
         <v>1</v>
       </c>
       <c r="T11" s="5">
@@ -7729,7 +7847,7 @@
       <c r="R12" s="7">
         <v>90</v>
       </c>
-      <c r="S12" s="5">
+      <c r="S12" s="18">
         <v>1</v>
       </c>
       <c r="T12" s="5">
@@ -7883,7 +8001,7 @@
       <c r="R13" s="7">
         <v>10</v>
       </c>
-      <c r="S13" s="5">
+      <c r="S13" s="18">
         <v>1</v>
       </c>
       <c r="T13" s="5">
@@ -8037,7 +8155,7 @@
       <c r="R14" s="7">
         <v>15</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S14" s="18">
         <v>1</v>
       </c>
       <c r="T14" s="5">
@@ -8193,7 +8311,7 @@
       <c r="R15" s="7">
         <v>4</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S15" s="18">
         <v>1</v>
       </c>
       <c r="T15" s="5">
@@ -8361,7 +8479,7 @@
       <c r="R16" s="7">
         <v>8</v>
       </c>
-      <c r="S16" s="5">
+      <c r="S16" s="18">
         <v>1</v>
       </c>
       <c r="T16" s="5">
@@ -8533,7 +8651,7 @@
       <c r="R17" s="7">
         <v>9</v>
       </c>
-      <c r="S17" s="5">
+      <c r="S17" s="18">
         <v>1</v>
       </c>
       <c r="T17" s="5">
@@ -8701,7 +8819,7 @@
       <c r="R18" s="7">
         <v>4</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="18">
         <v>1</v>
       </c>
       <c r="T18" s="5">
@@ -8867,7 +8985,7 @@
       <c r="R19" s="7">
         <v>5</v>
       </c>
-      <c r="S19" s="5">
+      <c r="S19" s="18">
         <v>1</v>
       </c>
       <c r="T19" s="5">
@@ -9019,7 +9137,7 @@
         <v>10</v>
       </c>
       <c r="R20" s="7"/>
-      <c r="S20" s="5">
+      <c r="S20" s="18">
         <v>1</v>
       </c>
       <c r="T20" s="5">
@@ -9177,7 +9295,7 @@
         <v>4</v>
       </c>
       <c r="R21" s="7"/>
-      <c r="S21" s="5">
+      <c r="S21" s="18">
         <v>1</v>
       </c>
       <c r="T21" s="5">
@@ -9339,7 +9457,7 @@
       <c r="R22" s="7">
         <v>10</v>
       </c>
-      <c r="S22" s="5">
+      <c r="S22" s="18">
         <v>1</v>
       </c>
       <c r="T22" s="5">
@@ -9505,7 +9623,7 @@
       <c r="R23" s="7">
         <v>90</v>
       </c>
-      <c r="S23" s="5">
+      <c r="S23" s="18">
         <v>1</v>
       </c>
       <c r="T23" s="5">
@@ -9655,7 +9773,7 @@
       <c r="R24" s="7">
         <v>10</v>
       </c>
-      <c r="S24" s="5">
+      <c r="S24" s="18">
         <v>1</v>
       </c>
       <c r="T24" s="5">
@@ -9811,7 +9929,7 @@
       <c r="R25" s="7">
         <v>71</v>
       </c>
-      <c r="S25" s="5">
+      <c r="S25" s="18">
         <v>1</v>
       </c>
       <c r="T25" s="5">
@@ -9969,7 +10087,7 @@
         <v>18</v>
       </c>
       <c r="R26" s="7"/>
-      <c r="S26" s="5">
+      <c r="S26" s="18">
         <v>1</v>
       </c>
       <c r="T26" s="5">
@@ -10119,7 +10237,7 @@
         <v>10</v>
       </c>
       <c r="R27" s="7"/>
-      <c r="S27" s="5">
+      <c r="S27" s="18">
         <v>1</v>
       </c>
       <c r="T27" s="5">
@@ -10291,7 +10409,7 @@
       <c r="R28" s="7">
         <v>1</v>
       </c>
-      <c r="S28" s="5">
+      <c r="S28" s="18">
         <v>1</v>
       </c>
       <c r="T28" s="5">
@@ -10459,7 +10577,7 @@
         <v>1</v>
       </c>
       <c r="R29" s="7"/>
-      <c r="S29" s="5">
+      <c r="S29" s="18">
         <v>1</v>
       </c>
       <c r="T29" s="5">
@@ -10635,7 +10753,7 @@
       <c r="R30" s="7">
         <v>10</v>
       </c>
-      <c r="S30" s="5">
+      <c r="S30" s="18">
         <v>1</v>
       </c>
       <c r="T30" s="5">
@@ -10801,7 +10919,7 @@
       <c r="R31" s="7">
         <v>7</v>
       </c>
-      <c r="S31" s="5">
+      <c r="S31" s="18">
         <v>1</v>
       </c>
       <c r="T31" s="5">
@@ -10963,7 +11081,7 @@
         <v>2</v>
       </c>
       <c r="R32" s="7"/>
-      <c r="S32" s="5">
+      <c r="S32" s="18">
         <v>1</v>
       </c>
       <c r="T32" s="5">
@@ -11125,7 +11243,7 @@
         <v>11</v>
       </c>
       <c r="R33" s="7"/>
-      <c r="S33" s="5">
+      <c r="S33" s="18">
         <v>1</v>
       </c>
       <c r="T33" s="5">
@@ -11267,7 +11385,7 @@
         <v>10</v>
       </c>
       <c r="R34" s="7"/>
-      <c r="S34" s="5">
+      <c r="S34" s="18">
         <v>1</v>
       </c>
       <c r="T34" s="5">
@@ -11417,7 +11535,7 @@
       <c r="R35" s="7">
         <v>24</v>
       </c>
-      <c r="S35" s="5">
+      <c r="S35" s="18">
         <v>1</v>
       </c>
       <c r="T35" s="5">
@@ -11567,7 +11685,7 @@
       <c r="R36" s="7">
         <v>24</v>
       </c>
-      <c r="S36" s="5">
+      <c r="S36" s="18">
         <v>1</v>
       </c>
       <c r="T36" s="5">
@@ -11725,7 +11843,7 @@
       <c r="R37" s="7">
         <v>18</v>
       </c>
-      <c r="S37" s="5">
+      <c r="S37" s="18">
         <v>1</v>
       </c>
       <c r="T37" s="5">
@@ -11879,7 +11997,7 @@
       <c r="R38" s="7">
         <v>28</v>
       </c>
-      <c r="S38" s="5">
+      <c r="S38" s="18">
         <v>1</v>
       </c>
       <c r="T38" s="5">
@@ -12031,7 +12149,7 @@
       <c r="R39" s="7">
         <v>17</v>
       </c>
-      <c r="S39" s="5">
+      <c r="S39" s="18">
         <v>1</v>
       </c>
       <c r="T39" s="5">
@@ -12189,7 +12307,7 @@
       <c r="R40" s="7">
         <v>10</v>
       </c>
-      <c r="S40" s="5">
+      <c r="S40" s="18">
         <v>1</v>
       </c>
       <c r="T40" s="5">
@@ -12343,7 +12461,7 @@
       <c r="R41" s="7">
         <v>10</v>
       </c>
-      <c r="S41" s="5">
+      <c r="S41" s="18">
         <v>1</v>
       </c>
       <c r="T41" s="5">
@@ -12503,7 +12621,7 @@
       <c r="R42" s="7">
         <v>2</v>
       </c>
-      <c r="S42" s="5">
+      <c r="S42" s="18">
         <v>1</v>
       </c>
       <c r="T42" s="5">
@@ -12653,7 +12771,7 @@
         <v>10</v>
       </c>
       <c r="R43" s="7"/>
-      <c r="S43" s="5">
+      <c r="S43" s="18">
         <v>1</v>
       </c>
       <c r="T43" s="5">
@@ -12805,7 +12923,7 @@
       <c r="R44" s="7">
         <v>2</v>
       </c>
-      <c r="S44" s="5">
+      <c r="S44" s="18">
         <v>1</v>
       </c>
       <c r="T44" s="5">
@@ -12971,7 +13089,7 @@
       <c r="R45" s="7">
         <v>5</v>
       </c>
-      <c r="S45" s="5">
+      <c r="S45" s="18">
         <v>1</v>
       </c>
       <c r="T45" s="5">
@@ -13123,7 +13241,7 @@
       <c r="R46" s="7">
         <v>7</v>
       </c>
-      <c r="S46" s="5">
+      <c r="S46" s="18">
         <v>1</v>
       </c>
       <c r="T46" s="5">
@@ -13271,7 +13389,7 @@
       </c>
       <c r="Q47" s="7"/>
       <c r="R47" s="7"/>
-      <c r="S47" s="5">
+      <c r="S47" s="18">
         <v>1</v>
       </c>
       <c r="T47" s="5">
@@ -13425,7 +13543,7 @@
         <v>3</v>
       </c>
       <c r="R48" s="7"/>
-      <c r="S48" s="5">
+      <c r="S48" s="18">
         <v>1</v>
       </c>
       <c r="T48" s="5">
@@ -13593,7 +13711,7 @@
       <c r="R49" s="7">
         <v>3</v>
       </c>
-      <c r="S49" s="5">
+      <c r="S49" s="18">
         <v>1</v>
       </c>
       <c r="T49" s="5">
@@ -13745,7 +13863,7 @@
       </c>
       <c r="Q50" s="7"/>
       <c r="R50" s="7"/>
-      <c r="S50" s="5">
+      <c r="S50" s="18">
         <v>1</v>
       </c>
       <c r="T50" s="5">
@@ -13901,7 +14019,7 @@
       <c r="R51" s="7">
         <v>10</v>
       </c>
-      <c r="S51" s="5">
+      <c r="S51" s="18">
         <v>1</v>
       </c>
       <c r="T51" s="5">
@@ -14051,7 +14169,7 @@
       <c r="R52" s="7">
         <v>3</v>
       </c>
-      <c r="S52" s="5">
+      <c r="S52" s="18">
         <v>1</v>
       </c>
       <c r="T52" s="5">
@@ -14205,7 +14323,7 @@
       <c r="R53" s="7">
         <v>3</v>
       </c>
-      <c r="S53" s="5">
+      <c r="S53" s="18">
         <v>1</v>
       </c>
       <c r="T53" s="5">
@@ -14361,7 +14479,7 @@
       <c r="R54" s="7">
         <v>2</v>
       </c>
-      <c r="S54" s="5">
+      <c r="S54" s="18">
         <v>1</v>
       </c>
       <c r="T54" s="5">
@@ -14515,7 +14633,7 @@
         <v>10</v>
       </c>
       <c r="R55" s="7"/>
-      <c r="S55" s="5">
+      <c r="S55" s="18">
         <v>1</v>
       </c>
       <c r="T55" s="5">
@@ -14677,7 +14795,7 @@
         <v>10</v>
       </c>
       <c r="R56" s="7"/>
-      <c r="S56" s="5">
+      <c r="S56" s="18">
         <v>1</v>
       </c>
       <c r="T56" s="5">
@@ -14833,7 +14951,7 @@
       <c r="R57" s="7">
         <v>6</v>
       </c>
-      <c r="S57" s="5">
+      <c r="S57" s="18">
         <v>1</v>
       </c>
       <c r="T57" s="5">
@@ -14987,7 +15105,7 @@
       <c r="R58" s="7">
         <v>2</v>
       </c>
-      <c r="S58" s="5">
+      <c r="S58" s="18">
         <v>1</v>
       </c>
       <c r="T58" s="5">
@@ -15137,7 +15255,7 @@
       </c>
       <c r="Q59" s="7"/>
       <c r="R59" s="7"/>
-      <c r="S59" s="5">
+      <c r="S59" s="18">
         <v>1</v>
       </c>
       <c r="T59" s="5">
@@ -15287,7 +15405,7 @@
       <c r="R60" s="7">
         <v>3</v>
       </c>
-      <c r="S60" s="5">
+      <c r="S60" s="18">
         <v>1</v>
       </c>
       <c r="T60" s="5">
@@ -15439,7 +15557,7 @@
         <v>2</v>
       </c>
       <c r="R61" s="7"/>
-      <c r="S61" s="5">
+      <c r="S61" s="18">
         <v>1</v>
       </c>
       <c r="T61" s="5">
@@ -15595,7 +15713,7 @@
       </c>
       <c r="Q62" s="7"/>
       <c r="R62" s="7"/>
-      <c r="S62" s="5">
+      <c r="S62" s="18">
         <v>1</v>
       </c>
       <c r="T62" s="5">
@@ -15751,7 +15869,7 @@
       <c r="R63" s="7">
         <v>7</v>
       </c>
-      <c r="S63" s="5">
+      <c r="S63" s="18">
         <v>1</v>
       </c>
       <c r="T63" s="5">
@@ -15911,7 +16029,7 @@
       <c r="R64" s="7">
         <v>15</v>
       </c>
-      <c r="S64" s="5">
+      <c r="S64" s="18">
         <v>1</v>
       </c>
       <c r="T64" s="5">
@@ -16089,7 +16207,7 @@
       <c r="R65" s="7">
         <v>1</v>
       </c>
-      <c r="S65" s="5">
+      <c r="S65" s="18">
         <v>1</v>
       </c>
       <c r="T65" s="5">
@@ -16261,7 +16379,7 @@
       <c r="P66" s="7"/>
       <c r="Q66" s="7"/>
       <c r="R66" s="7"/>
-      <c r="S66" s="5">
+      <c r="S66" s="18">
         <v>1</v>
       </c>
       <c r="T66" s="5">
@@ -16425,7 +16543,7 @@
         <v>2</v>
       </c>
       <c r="R67" s="7"/>
-      <c r="S67" s="5">
+      <c r="S67" s="18">
         <v>1</v>
       </c>
       <c r="T67" s="5">
@@ -16591,7 +16709,7 @@
       <c r="R68" s="7">
         <v>6</v>
       </c>
-      <c r="S68" s="5">
+      <c r="S68" s="18">
         <v>1</v>
       </c>
       <c r="T68" s="5">
@@ -16745,7 +16863,7 @@
       <c r="R69" s="7">
         <v>2</v>
       </c>
-      <c r="S69" s="5">
+      <c r="S69" s="18">
         <v>1</v>
       </c>
       <c r="T69" s="5">
@@ -16893,7 +17011,7 @@
       <c r="R70" s="7">
         <v>2</v>
       </c>
-      <c r="S70" s="5">
+      <c r="S70" s="18">
         <v>1</v>
       </c>
       <c r="T70" s="5">
@@ -17024,7 +17142,7 @@
         <v>589</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>983</v>
+        <v>1038</v>
       </c>
       <c r="J71" s="11" t="s">
         <v>612</v>
@@ -17043,7 +17161,7 @@
       <c r="R71" s="7">
         <v>10</v>
       </c>
-      <c r="S71" s="5">
+      <c r="S71" s="18">
         <v>0.01</v>
       </c>
       <c r="T71" s="5">
@@ -17119,7 +17237,7 @@
       </c>
       <c r="BC71" s="13" t="str" cm="1">
         <f t="array" ref="BC71">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val mina = 69("mina", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFFFF84, 0xFFFF00, 0xFFFF00, 0xFFC800))</v>
+        <v>val mina = 69("mina", { null }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFFFF84, 0xFFFF00, 0xFFFF00, 0xFFC800))</v>
       </c>
       <c r="BD71" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
@@ -17185,7 +17303,7 @@
       <c r="R72" s="7">
         <v>95</v>
       </c>
-      <c r="S72" s="5">
+      <c r="S72" s="18">
         <v>1</v>
       </c>
       <c r="T72" s="5">
@@ -17345,7 +17463,7 @@
       <c r="R73" s="7">
         <v>83</v>
       </c>
-      <c r="S73" s="5">
+      <c r="S73" s="18">
         <v>1</v>
       </c>
       <c r="T73" s="5">
@@ -17511,7 +17629,7 @@
       <c r="R74" s="7">
         <v>63</v>
       </c>
-      <c r="S74" s="5">
+      <c r="S74" s="18">
         <v>1</v>
       </c>
       <c r="T74" s="5">
@@ -17677,7 +17795,7 @@
       <c r="R75" s="7">
         <v>70</v>
       </c>
-      <c r="S75" s="5">
+      <c r="S75" s="18">
         <v>1</v>
       </c>
       <c r="T75" s="5">
@@ -17839,7 +17957,7 @@
       <c r="R76" s="7">
         <v>64</v>
       </c>
-      <c r="S76" s="5">
+      <c r="S76" s="18">
         <v>1</v>
       </c>
       <c r="T76" s="5">
@@ -18001,7 +18119,7 @@
       <c r="R77" s="7">
         <v>43</v>
       </c>
-      <c r="S77" s="5">
+      <c r="S77" s="18">
         <v>1</v>
       </c>
       <c r="T77" s="5">
@@ -18161,7 +18279,7 @@
       <c r="R78" s="7">
         <v>75</v>
       </c>
-      <c r="S78" s="5">
+      <c r="S78" s="18">
         <v>1</v>
       </c>
       <c r="T78" s="5">
@@ -18319,7 +18437,7 @@
       <c r="R79" s="7">
         <v>85</v>
       </c>
-      <c r="S79" s="5">
+      <c r="S79" s="18">
         <v>1</v>
       </c>
       <c r="T79" s="5">
@@ -18477,7 +18595,7 @@
       <c r="R80" s="7">
         <v>7</v>
       </c>
-      <c r="S80" s="5">
+      <c r="S80" s="18">
         <v>1.2</v>
       </c>
       <c r="T80" s="5">
@@ -18637,7 +18755,7 @@
       <c r="R81" s="7">
         <v>5</v>
       </c>
-      <c r="S81" s="5">
+      <c r="S81" s="18">
         <v>1.2</v>
       </c>
       <c r="T81" s="5">
@@ -18821,7 +18939,7 @@
       <c r="R82" s="7">
         <v>98</v>
       </c>
-      <c r="S82" s="5">
+      <c r="S82" s="18">
         <v>1</v>
       </c>
       <c r="T82" s="5">
@@ -18981,7 +19099,7 @@
         <v>63</v>
       </c>
       <c r="R83" s="7"/>
-      <c r="S83" s="5">
+      <c r="S83" s="18">
         <v>1</v>
       </c>
       <c r="T83" s="5">
@@ -19141,7 +19259,7 @@
       <c r="R84" s="7">
         <v>1</v>
       </c>
-      <c r="S84" s="5">
+      <c r="S84" s="18">
         <v>1</v>
       </c>
       <c r="T84" s="5">
@@ -19307,7 +19425,7 @@
       <c r="R85" s="7">
         <v>3</v>
       </c>
-      <c r="S85" s="5">
+      <c r="S85" s="18">
         <v>1</v>
       </c>
       <c r="T85" s="5">
@@ -19467,7 +19585,7 @@
       </c>
       <c r="Q86" s="7"/>
       <c r="R86" s="7"/>
-      <c r="S86" s="5">
+      <c r="S86" s="18">
         <v>1</v>
       </c>
       <c r="T86" s="5">
@@ -19619,7 +19737,7 @@
       <c r="R87" s="7">
         <v>12</v>
       </c>
-      <c r="S87" s="5">
+      <c r="S87" s="18">
         <v>1</v>
       </c>
       <c r="T87" s="5">
@@ -19767,7 +19885,7 @@
       <c r="R88" s="7">
         <v>10</v>
       </c>
-      <c r="S88" s="5">
+      <c r="S88" s="18">
         <v>1</v>
       </c>
       <c r="T88" s="5">
@@ -19935,7 +20053,7 @@
       <c r="R89" s="7">
         <v>10</v>
       </c>
-      <c r="S89" s="5">
+      <c r="S89" s="18">
         <v>1</v>
       </c>
       <c r="T89" s="5">
@@ -20095,7 +20213,7 @@
       <c r="R90" s="7">
         <v>10</v>
       </c>
-      <c r="S90" s="5">
+      <c r="S90" s="18">
         <v>1</v>
       </c>
       <c r="T90" s="5">
@@ -20267,7 +20385,7 @@
       <c r="R91" s="7">
         <v>10</v>
       </c>
-      <c r="S91" s="5">
+      <c r="S91" s="18">
         <v>1</v>
       </c>
       <c r="T91" s="5">
@@ -20417,7 +20535,7 @@
       <c r="R92" s="7">
         <v>17</v>
       </c>
-      <c r="S92" s="5">
+      <c r="S92" s="18">
         <v>1</v>
       </c>
       <c r="T92" s="5">
@@ -20573,7 +20691,7 @@
       <c r="R93" s="7">
         <v>42</v>
       </c>
-      <c r="S93" s="5">
+      <c r="S93" s="18">
         <v>1</v>
       </c>
       <c r="T93" s="5">
@@ -20743,7 +20861,7 @@
       <c r="R94" s="7">
         <v>35</v>
       </c>
-      <c r="S94" s="5">
+      <c r="S94" s="18">
         <v>1</v>
       </c>
       <c r="T94" s="5">
@@ -20905,7 +21023,7 @@
       <c r="R95" s="7">
         <v>5</v>
       </c>
-      <c r="S95" s="5">
+      <c r="S95" s="18">
         <v>1</v>
       </c>
       <c r="T95" s="5">
@@ -21069,7 +21187,7 @@
       <c r="R96" s="7">
         <v>6</v>
       </c>
-      <c r="S96" s="5">
+      <c r="S96" s="18">
         <v>1</v>
       </c>
       <c r="T96" s="5">
@@ -21231,7 +21349,7 @@
         <v>10</v>
       </c>
       <c r="R97" s="7"/>
-      <c r="S97" s="5">
+      <c r="S97" s="18">
         <v>1</v>
       </c>
       <c r="T97" s="5">
@@ -21385,7 +21503,7 @@
         <v>10</v>
       </c>
       <c r="R98" s="7"/>
-      <c r="S98" s="5">
+      <c r="S98" s="18">
         <v>1</v>
       </c>
       <c r="T98" s="5">
@@ -21537,7 +21655,7 @@
         <v>10</v>
       </c>
       <c r="R99" s="7"/>
-      <c r="S99" s="5">
+      <c r="S99" s="18">
         <v>1</v>
       </c>
       <c r="T99" s="5">
@@ -21691,7 +21809,7 @@
       <c r="R100" s="7">
         <v>8</v>
       </c>
-      <c r="S100" s="5">
+      <c r="S100" s="18">
         <v>1.5</v>
       </c>
       <c r="T100" s="5">
@@ -21847,7 +21965,7 @@
       <c r="R101" s="7">
         <v>21</v>
       </c>
-      <c r="S101" s="5">
+      <c r="S101" s="18">
         <v>1</v>
       </c>
       <c r="T101" s="5">
@@ -21999,7 +22117,7 @@
       <c r="P102" s="7"/>
       <c r="Q102" s="7"/>
       <c r="R102" s="7"/>
-      <c r="S102" s="5">
+      <c r="S102" s="18">
         <v>1</v>
       </c>
       <c r="T102" s="5">
@@ -22153,7 +22271,7 @@
       <c r="R103" s="7">
         <v>12</v>
       </c>
-      <c r="S103" s="5">
+      <c r="S103" s="18">
         <v>1</v>
       </c>
       <c r="T103" s="5">
@@ -22305,7 +22423,7 @@
         <v>10</v>
       </c>
       <c r="R104" s="7"/>
-      <c r="S104" s="5">
+      <c r="S104" s="18">
         <v>1</v>
       </c>
       <c r="T104" s="5">
@@ -22465,7 +22583,7 @@
       <c r="R105" s="7">
         <v>1</v>
       </c>
-      <c r="S105" s="5">
+      <c r="S105" s="18">
         <v>1</v>
       </c>
       <c r="T105" s="5">
@@ -22619,7 +22737,7 @@
       <c r="R106" s="7">
         <v>7</v>
       </c>
-      <c r="S106" s="5">
+      <c r="S106" s="18">
         <v>1</v>
       </c>
       <c r="T106" s="5">
@@ -22767,7 +22885,7 @@
       <c r="R107" s="7">
         <v>9</v>
       </c>
-      <c r="S107" s="5">
+      <c r="S107" s="18">
         <v>1</v>
       </c>
       <c r="T107" s="5">
@@ -22917,7 +23035,7 @@
       <c r="R108" s="7">
         <v>3</v>
       </c>
-      <c r="S108" s="5">
+      <c r="S108" s="18">
         <v>1</v>
       </c>
       <c r="T108" s="5">
@@ -23065,7 +23183,7 @@
       <c r="R109" s="7">
         <v>5</v>
       </c>
-      <c r="S109" s="5">
+      <c r="S109" s="18">
         <v>1</v>
       </c>
       <c r="T109" s="5">
@@ -23215,7 +23333,7 @@
         <v>10</v>
       </c>
       <c r="R110" s="7"/>
-      <c r="S110" s="5">
+      <c r="S110" s="18">
         <v>1</v>
       </c>
       <c r="T110" s="5">
@@ -23369,7 +23487,7 @@
         <v>41</v>
       </c>
       <c r="R111" s="7"/>
-      <c r="S111" s="5">
+      <c r="S111" s="18">
         <v>1.2</v>
       </c>
       <c r="T111" s="5">
@@ -23543,7 +23661,7 @@
       <c r="R112" s="7">
         <v>3</v>
       </c>
-      <c r="S112" s="5">
+      <c r="S112" s="18">
         <v>1</v>
       </c>
       <c r="T112" s="5">
@@ -23705,7 +23823,7 @@
         <v>10</v>
       </c>
       <c r="R113" s="7"/>
-      <c r="S113" s="5">
+      <c r="S113" s="18">
         <v>1</v>
       </c>
       <c r="T113" s="5">
@@ -23879,7 +23997,7 @@
       <c r="R114" s="7">
         <v>3</v>
       </c>
-      <c r="S114" s="5">
+      <c r="S114" s="18">
         <v>1</v>
       </c>
       <c r="T114" s="5">
@@ -24037,7 +24155,7 @@
       <c r="P115" s="7"/>
       <c r="Q115" s="7"/>
       <c r="R115" s="7"/>
-      <c r="S115" s="5">
+      <c r="S115" s="18">
         <v>1</v>
       </c>
       <c r="T115" s="5">
@@ -24201,7 +24319,7 @@
       </c>
       <c r="Q116" s="7"/>
       <c r="R116" s="7"/>
-      <c r="S116" s="5">
+      <c r="S116" s="18">
         <v>1</v>
       </c>
       <c r="T116" s="5">
@@ -24367,7 +24485,7 @@
         <v>10</v>
       </c>
       <c r="R117" s="7"/>
-      <c r="S117" s="5">
+      <c r="S117" s="18">
         <v>1</v>
       </c>
       <c r="T117" s="5">
@@ -24531,7 +24649,7 @@
       <c r="R118" s="7">
         <v>1</v>
       </c>
-      <c r="S118" s="5">
+      <c r="S118" s="18">
         <v>1</v>
       </c>
       <c r="T118" s="5">
@@ -24685,7 +24803,7 @@
         <v>10</v>
       </c>
       <c r="R119" s="7"/>
-      <c r="S119" s="5">
+      <c r="S119" s="18">
         <v>1</v>
       </c>
       <c r="T119" s="5">
@@ -24841,7 +24959,7 @@
         <v>10</v>
       </c>
       <c r="R120" s="7"/>
-      <c r="S120" s="5">
+      <c r="S120" s="18">
         <v>1</v>
       </c>
       <c r="T120" s="5">
@@ -25005,7 +25123,7 @@
         <v>26</v>
       </c>
       <c r="R121" s="7"/>
-      <c r="S121" s="5">
+      <c r="S121" s="18">
         <v>1.2</v>
       </c>
       <c r="T121" s="5">
@@ -25169,7 +25287,7 @@
       <c r="R122" s="7">
         <v>5</v>
       </c>
-      <c r="S122" s="5">
+      <c r="S122" s="18">
         <v>1</v>
       </c>
       <c r="T122" s="5">
@@ -25321,7 +25439,7 @@
       <c r="R123" s="7">
         <v>1</v>
       </c>
-      <c r="S123" s="5">
+      <c r="S123" s="18">
         <v>1</v>
       </c>
       <c r="T123" s="5">
@@ -25473,7 +25591,7 @@
       <c r="R124" s="7">
         <v>1</v>
       </c>
-      <c r="S124" s="5">
+      <c r="S124" s="18">
         <v>1</v>
       </c>
       <c r="T124" s="5">
@@ -25627,7 +25745,7 @@
       </c>
       <c r="Q125" s="7"/>
       <c r="R125" s="7"/>
-      <c r="S125" s="5">
+      <c r="S125" s="18">
         <v>1</v>
       </c>
       <c r="T125" s="5">
@@ -25783,7 +25901,7 @@
       <c r="R126" s="7">
         <v>5</v>
       </c>
-      <c r="S126" s="5">
+      <c r="S126" s="18">
         <v>1</v>
       </c>
       <c r="T126" s="5">
@@ -25943,7 +26061,7 @@
       <c r="R127" s="7">
         <v>3</v>
       </c>
-      <c r="S127" s="5">
+      <c r="S127" s="18">
         <v>1</v>
       </c>
       <c r="T127" s="5">
@@ -26099,7 +26217,7 @@
         <v>10</v>
       </c>
       <c r="R128" s="7"/>
-      <c r="S128" s="5">
+      <c r="S128" s="18">
         <v>1</v>
       </c>
       <c r="T128" s="5">
@@ -26253,7 +26371,7 @@
         <v>10</v>
       </c>
       <c r="R129" s="7"/>
-      <c r="S129" s="5">
+      <c r="S129" s="18">
         <v>1</v>
       </c>
       <c r="T129" s="5">
@@ -26423,7 +26541,7 @@
       <c r="R130" s="7">
         <v>21</v>
       </c>
-      <c r="S130" s="5">
+      <c r="S130" s="18">
         <v>1</v>
       </c>
       <c r="T130" s="5">
@@ -26579,7 +26697,7 @@
         <v>13</v>
       </c>
       <c r="R131" s="7"/>
-      <c r="S131" s="5">
+      <c r="S131" s="18">
         <v>1.2</v>
       </c>
       <c r="T131" s="5">
@@ -26737,7 +26855,7 @@
       <c r="R132" s="7">
         <v>10</v>
       </c>
-      <c r="S132" s="5">
+      <c r="S132" s="18">
         <v>1</v>
       </c>
       <c r="T132" s="5">
@@ -26911,7 +27029,7 @@
         <v>9</v>
       </c>
       <c r="R133" s="7"/>
-      <c r="S133" s="5">
+      <c r="S133" s="18">
         <v>1</v>
       </c>
       <c r="T133" s="5">
@@ -27081,7 +27199,7 @@
       <c r="R134" s="7">
         <v>3</v>
       </c>
-      <c r="S134" s="5">
+      <c r="S134" s="18">
         <v>1</v>
       </c>
       <c r="T134" s="5">
@@ -27239,7 +27357,7 @@
         <v>10</v>
       </c>
       <c r="R135" s="7"/>
-      <c r="S135" s="5">
+      <c r="S135" s="18">
         <v>1</v>
       </c>
       <c r="T135" s="5">
@@ -27395,7 +27513,7 @@
       <c r="R136" s="7">
         <v>4</v>
       </c>
-      <c r="S136" s="5">
+      <c r="S136" s="18">
         <v>1</v>
       </c>
       <c r="T136" s="5">
@@ -27549,7 +27667,7 @@
         <v>13</v>
       </c>
       <c r="R137" s="7"/>
-      <c r="S137" s="5">
+      <c r="S137" s="18">
         <v>1</v>
       </c>
       <c r="T137" s="5">
@@ -27705,7 +27823,7 @@
       </c>
       <c r="Q138" s="7"/>
       <c r="R138" s="7"/>
-      <c r="S138" s="5">
+      <c r="S138" s="18">
         <v>1</v>
       </c>
       <c r="T138" s="5">
@@ -27869,7 +27987,7 @@
       <c r="R139" s="7">
         <v>1</v>
       </c>
-      <c r="S139" s="5">
+      <c r="S139" s="18">
         <v>1</v>
       </c>
       <c r="T139" s="5">
@@ -28031,7 +28149,7 @@
       <c r="R140" s="7">
         <v>14</v>
       </c>
-      <c r="S140" s="5">
+      <c r="S140" s="18">
         <v>1</v>
       </c>
       <c r="T140" s="5">
@@ -28191,7 +28309,7 @@
       <c r="R141" s="7">
         <v>5</v>
       </c>
-      <c r="S141" s="5">
+      <c r="S141" s="18">
         <v>1</v>
       </c>
       <c r="T141" s="5">
@@ -28305,42 +28423,52 @@
       <c r="B142" s="4">
         <v>1</v>
       </c>
-      <c r="C142" s="4"/>
-      <c r="D142" s="4"/>
+      <c r="C142" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D142" s="4" t="s">
+        <v>552</v>
+      </c>
       <c r="E142" s="6" t="s">
-        <v>1050</v>
+        <v>1056</v>
       </c>
       <c r="F142" s="6" t="s">
-        <v>1038</v>
+        <v>1055</v>
       </c>
       <c r="G142" s="6" t="s">
-        <v>1038</v>
+        <v>1071</v>
       </c>
       <c r="H142" s="6" t="s">
-        <v>1038</v>
+        <v>1078</v>
       </c>
       <c r="I142" s="6" t="s">
         <v>983</v>
       </c>
       <c r="J142" s="11" t="s">
-        <v>1057</v>
+        <v>1090</v>
       </c>
       <c r="K142" s="3">
         <v>1</v>
       </c>
       <c r="L142" s="8">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="M142" s="7"/>
-      <c r="N142" s="7"/>
+      <c r="N142" s="7">
+        <v>10</v>
+      </c>
       <c r="O142" s="7"/>
-      <c r="P142" s="7"/>
-      <c r="Q142" s="7"/>
+      <c r="P142" s="7">
+        <v>8</v>
+      </c>
+      <c r="Q142" s="7">
+        <v>3</v>
+      </c>
       <c r="R142" s="7">
-        <v>10</v>
-      </c>
-      <c r="S142" s="5">
-        <v>0.01</v>
+        <v>5</v>
+      </c>
+      <c r="S142" s="18">
+        <v>1</v>
       </c>
       <c r="T142" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
@@ -28348,15 +28476,15 @@
       </c>
       <c r="U142" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M142:R142)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.80106987758962211</v>
       </c>
       <c r="V142" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>0.80106987758962211</v>
       </c>
       <c r="W142" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>17.623537306971688</v>
       </c>
       <c r="X142" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -28364,7 +28492,7 @@
       </c>
       <c r="Y142" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>6.7782835796044951</v>
       </c>
       <c r="Z142" s="9">
         <f>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -28372,24 +28500,28 @@
       </c>
       <c r="AA142" s="9">
         <f>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>5.4226268636835959</v>
       </c>
       <c r="AB142" s="9">
         <f>テーブル1[[#This Row],[基礎Aqua]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>2.0334850738813488</v>
       </c>
       <c r="AC142" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
+        <v>3.3891417898022476</v>
       </c>
       <c r="AD142" s="14"/>
-      <c r="AE142" s="14"/>
+      <c r="AE142" s="14">
+        <v>1</v>
+      </c>
       <c r="AF142" s="14"/>
       <c r="AG142" s="14"/>
       <c r="AH142" s="14"/>
       <c r="AI142" s="14"/>
       <c r="AJ142" s="14"/>
-      <c r="AK142" s="14"/>
+      <c r="AK142" s="14">
+        <v>3</v>
+      </c>
       <c r="AL142" s="14"/>
       <c r="AM142" s="14"/>
       <c r="AN142" s="14"/>
@@ -28397,37 +28529,45 @@
       <c r="AP142" s="14"/>
       <c r="AQ142" s="14"/>
       <c r="AR142" s="14"/>
-      <c r="AS142" s="14"/>
+      <c r="AS142" s="14">
+        <v>4</v>
+      </c>
       <c r="AT142" s="14"/>
-      <c r="AU142" s="14"/>
+      <c r="AU142" s="14">
+        <v>1</v>
+      </c>
       <c r="AV142" s="14"/>
       <c r="AW142" s="14"/>
-      <c r="AX142" s="14"/>
+      <c r="AX142" s="14">
+        <v>8</v>
+      </c>
       <c r="AY142" s="14"/>
-      <c r="AZ142" s="14"/>
+      <c r="AZ142" s="14">
+        <v>10</v>
+      </c>
       <c r="BA142" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="BB142" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null140</v>
+        <v>button</v>
       </c>
       <c r="BC142" s="13" t="str" cm="1">
         <f t="array" ref="BC142">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null140 = 140("null140", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000000))</v>
+        <v>val button = 140("button", { mirage }, 1, 22, 1.00, m(0.0, 10.0, 0.0, 8.0, 3.0, 5.0), a(0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 3.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 4.0, 0.0, 1.0, 0.0, 0.0, 8.0, 0.0, 10.0), c(0xFFFFFF, 0xBC9862, 0xBC9862, 0xD40102))</v>
       </c>
       <c r="BD142" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null140.name=null</v>
+        <v>mirageFairy2019.fairy.button.name=Buttonia</v>
       </c>
       <c r="BE142" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null140.name=nullnull</v>
+        <v>mirageFairy2019.fairy.button.name=釦精ブットーニャ</v>
       </c>
       <c r="BF142" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
-        <v>0</v>
+        <v>0.40151190863491365</v>
       </c>
     </row>
     <row r="143" spans="1:58" x14ac:dyDescent="0.15">
@@ -28437,58 +28577,64 @@
       <c r="B143" s="4">
         <v>1</v>
       </c>
-      <c r="C143" s="4"/>
-      <c r="D143" s="4"/>
+      <c r="C143" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>551</v>
+      </c>
       <c r="E143" s="6" t="s">
-        <v>1051</v>
+        <v>1061</v>
       </c>
       <c r="F143" s="6" t="s">
-        <v>1038</v>
+        <v>1062</v>
       </c>
       <c r="G143" s="6" t="s">
-        <v>1038</v>
+        <v>1074</v>
       </c>
       <c r="H143" s="6" t="s">
-        <v>1038</v>
+        <v>1081</v>
       </c>
       <c r="I143" s="6" t="s">
-        <v>983</v>
+        <v>521</v>
       </c>
       <c r="J143" s="11" t="s">
-        <v>1058</v>
+        <v>1088</v>
       </c>
       <c r="K143" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L143" s="8">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="M143" s="7"/>
       <c r="N143" s="7"/>
       <c r="O143" s="7"/>
       <c r="P143" s="7"/>
-      <c r="Q143" s="7"/>
+      <c r="Q143" s="7">
+        <v>10</v>
+      </c>
       <c r="R143" s="7">
-        <v>10</v>
-      </c>
-      <c r="S143" s="5">
-        <v>0.01</v>
+        <v>2</v>
+      </c>
+      <c r="S143" s="18">
+        <v>1</v>
       </c>
       <c r="T143" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>1.189207115002721</v>
       </c>
       <c r="U143" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M143:R143)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.97265494741228553</v>
       </c>
       <c r="V143" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.1566881839052874</v>
       </c>
       <c r="W143" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>25.447140045916321</v>
       </c>
       <c r="X143" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -28508,18 +28654,22 @@
       </c>
       <c r="AB143" s="9">
         <f>テーブル1[[#This Row],[基礎Aqua]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>21.205950038263598</v>
       </c>
       <c r="AC143" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
+        <v>4.2411900076527198</v>
       </c>
       <c r="AD143" s="14"/>
-      <c r="AE143" s="14"/>
+      <c r="AE143" s="14">
+        <v>1</v>
+      </c>
       <c r="AF143" s="14"/>
       <c r="AG143" s="14"/>
       <c r="AH143" s="14"/>
-      <c r="AI143" s="14"/>
+      <c r="AI143" s="14">
+        <v>1</v>
+      </c>
       <c r="AJ143" s="14"/>
       <c r="AK143" s="14"/>
       <c r="AL143" s="14"/>
@@ -28528,9 +28678,13 @@
       <c r="AO143" s="14"/>
       <c r="AP143" s="14"/>
       <c r="AQ143" s="14"/>
-      <c r="AR143" s="14"/>
+      <c r="AR143" s="14">
+        <v>12</v>
+      </c>
       <c r="AS143" s="14"/>
-      <c r="AT143" s="14"/>
+      <c r="AT143" s="14">
+        <v>4</v>
+      </c>
       <c r="AU143" s="14"/>
       <c r="AV143" s="14"/>
       <c r="AW143" s="14"/>
@@ -28539,23 +28693,23 @@
       <c r="AZ143" s="14"/>
       <c r="BA143" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="BB143" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null141</v>
+        <v>cookedCod</v>
       </c>
       <c r="BC143" s="13" t="str" cm="1">
         <f t="array" ref="BC143">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null141 = 141("null141", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000001))</v>
+        <v>val cookedCod = 141("cooked_cod", { cod }, 2, 22, 1.00, m(0.0, 0.0, 0.0, 0.0, 10.0, 2.0), a(0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 12.0, 0.0, 4.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xC4B1B4, 0xC4B1B4, 0xC4B1B4, 0x6B9F93))</v>
       </c>
       <c r="BD143" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null141.name=null</v>
+        <v>mirageFairy2019.fairy.cooked_cod.name=Cookede Codia</v>
       </c>
       <c r="BE143" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null141.name=nullnull</v>
+        <v>mirageFairy2019.fairy.cooked_cod.name=焼鱈精ツォーケーデツォージャ</v>
       </c>
       <c r="BF143" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
@@ -28569,62 +28723,70 @@
       <c r="B144" s="4">
         <v>1</v>
       </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
+      <c r="C144" s="4" t="s">
+        <v>392</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>409</v>
+      </c>
       <c r="E144" s="6" t="s">
-        <v>1052</v>
+        <v>1063</v>
       </c>
       <c r="F144" s="6" t="s">
-        <v>1038</v>
+        <v>1064</v>
       </c>
       <c r="G144" s="6" t="s">
-        <v>1038</v>
+        <v>1082</v>
       </c>
       <c r="H144" s="6" t="s">
-        <v>1038</v>
+        <v>1083</v>
       </c>
       <c r="I144" s="6" t="s">
         <v>983</v>
       </c>
       <c r="J144" s="11" t="s">
-        <v>1059</v>
+        <v>1086</v>
       </c>
       <c r="K144" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L144" s="8">
-        <v>50</v>
-      </c>
-      <c r="M144" s="7"/>
+        <v>35</v>
+      </c>
+      <c r="M144" s="7">
+        <v>1</v>
+      </c>
       <c r="N144" s="7"/>
-      <c r="O144" s="7"/>
+      <c r="O144" s="7">
+        <v>3</v>
+      </c>
       <c r="P144" s="7"/>
-      <c r="Q144" s="7"/>
-      <c r="R144" s="7">
+      <c r="Q144" s="7">
         <v>10</v>
       </c>
-      <c r="S144" s="5">
-        <v>0.01</v>
+      <c r="R144" s="7"/>
+      <c r="S144" s="18">
+        <v>1</v>
       </c>
       <c r="T144" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="U144" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M144:R144)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.94605764672559589</v>
       </c>
       <c r="V144" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.337927554786112</v>
       </c>
       <c r="W144" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>46.827464417513923</v>
       </c>
       <c r="X144" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>3.3448188869652804</v>
       </c>
       <c r="Y144" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -28632,7 +28794,7 @@
       </c>
       <c r="Z144" s="9">
         <f>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>10.034456660895842</v>
       </c>
       <c r="AA144" s="9">
         <f>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -28640,54 +28802,72 @@
       </c>
       <c r="AB144" s="9">
         <f>テーブル1[[#This Row],[基礎Aqua]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>33.448188869652803</v>
       </c>
       <c r="AC144" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AD144" s="14"/>
       <c r="AE144" s="14"/>
-      <c r="AF144" s="14"/>
-      <c r="AG144" s="14"/>
+      <c r="AF144" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG144" s="14">
+        <v>4</v>
+      </c>
       <c r="AH144" s="14"/>
-      <c r="AI144" s="14"/>
+      <c r="AI144" s="14">
+        <v>2</v>
+      </c>
       <c r="AJ144" s="14"/>
       <c r="AK144" s="14"/>
       <c r="AL144" s="14"/>
       <c r="AM144" s="14"/>
       <c r="AN144" s="14"/>
       <c r="AO144" s="14"/>
-      <c r="AP144" s="14"/>
+      <c r="AP144" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ144" s="14"/>
-      <c r="AR144" s="14"/>
-      <c r="AS144" s="14"/>
-      <c r="AT144" s="14"/>
+      <c r="AR144" s="14">
+        <v>8</v>
+      </c>
+      <c r="AS144" s="14">
+        <v>8</v>
+      </c>
+      <c r="AT144" s="14">
+        <v>1</v>
+      </c>
       <c r="AU144" s="14"/>
       <c r="AV144" s="14"/>
       <c r="AW144" s="14"/>
       <c r="AX144" s="14"/>
-      <c r="AY144" s="14"/>
-      <c r="AZ144" s="14"/>
+      <c r="AY144" s="14">
+        <v>1</v>
+      </c>
+      <c r="AZ144" s="14">
+        <v>2</v>
+      </c>
       <c r="BA144" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="BB144" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null142</v>
+        <v>peony</v>
       </c>
       <c r="BC144" s="13" t="str" cm="1">
         <f t="array" ref="BC144">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null142 = 142("null142", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000002))</v>
+        <v>val peony = 142("peony", { mirage }, 3, 35, 1.00, m(1.0, 0.0, 3.0, 0.0, 10.0, 0.0), a(0.0, 0.0, 1.0, 4.0, 0.0, 2.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 8.0, 8.0, 1.0, 0.0, 0.0, 0.0, 0.0, 1.0, 2.0), c(0x63D700, 0xEDD6F7, 0xEDD6F7, 0xDEA5F7))</v>
       </c>
       <c r="BD144" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null142.name=null</v>
+        <v>mirageFairy2019.fairy.peony.name=Peonia</v>
       </c>
       <c r="BE144" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null142.name=nullnull</v>
+        <v>mirageFairy2019.fairy.peony.name=牡丹精ペオーニャ</v>
       </c>
       <c r="BF144" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
@@ -28701,101 +28881,127 @@
       <c r="B145" s="4">
         <v>1</v>
       </c>
-      <c r="C145" s="4"/>
-      <c r="D145" s="4"/>
+      <c r="C145" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>410</v>
+      </c>
       <c r="E145" s="6" t="s">
-        <v>1053</v>
+        <v>279</v>
       </c>
       <c r="F145" s="6" t="s">
-        <v>1038</v>
+        <v>1054</v>
       </c>
       <c r="G145" s="6" t="s">
-        <v>1038</v>
+        <v>1070</v>
       </c>
       <c r="H145" s="6" t="s">
-        <v>1038</v>
+        <v>1077</v>
       </c>
       <c r="I145" s="6" t="s">
         <v>983</v>
       </c>
       <c r="J145" s="11" t="s">
-        <v>1060</v>
+        <v>1087</v>
       </c>
       <c r="K145" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L145" s="8">
-        <v>50</v>
-      </c>
-      <c r="M145" s="7"/>
-      <c r="N145" s="7"/>
-      <c r="O145" s="7"/>
-      <c r="P145" s="7"/>
-      <c r="Q145" s="7"/>
+        <v>30</v>
+      </c>
+      <c r="M145" s="7">
+        <v>1</v>
+      </c>
+      <c r="N145" s="7">
+        <v>5</v>
+      </c>
+      <c r="O145" s="7">
+        <v>5</v>
+      </c>
+      <c r="P145" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q145" s="7">
+        <v>3</v>
+      </c>
       <c r="R145" s="7">
-        <v>10</v>
-      </c>
-      <c r="S145" s="5">
-        <v>0.01</v>
+        <v>2</v>
+      </c>
+      <c r="S145" s="18">
+        <v>1</v>
       </c>
       <c r="T145" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>1.4142135623730951</v>
       </c>
       <c r="U145" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M145:R145)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.80106987758962211</v>
       </c>
       <c r="V145" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.1328838852957988</v>
       </c>
       <c r="W145" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>33.986516558873966</v>
       </c>
       <c r="X145" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>1.3071737138028448</v>
       </c>
       <c r="Y145" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>6.5358685690142249</v>
       </c>
       <c r="Z145" s="9">
         <f>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>6.5358685690142249</v>
       </c>
       <c r="AA145" s="9">
         <f>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>13.07173713802845</v>
       </c>
       <c r="AB145" s="9">
         <f>テーブル1[[#This Row],[基礎Aqua]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>3.921521141408534</v>
       </c>
       <c r="AC145" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
-      </c>
-      <c r="AD145" s="14"/>
-      <c r="AE145" s="14"/>
+        <v>2.6143474276056895</v>
+      </c>
+      <c r="AD145" s="14">
+        <v>1</v>
+      </c>
+      <c r="AE145" s="14">
+        <v>3</v>
+      </c>
       <c r="AF145" s="14"/>
       <c r="AG145" s="14"/>
       <c r="AH145" s="14"/>
       <c r="AI145" s="14"/>
       <c r="AJ145" s="14"/>
-      <c r="AK145" s="14"/>
+      <c r="AK145" s="14">
+        <v>1</v>
+      </c>
       <c r="AL145" s="14"/>
       <c r="AM145" s="14"/>
       <c r="AN145" s="14"/>
-      <c r="AO145" s="14"/>
+      <c r="AO145" s="14">
+        <v>1</v>
+      </c>
       <c r="AP145" s="14"/>
       <c r="AQ145" s="14"/>
       <c r="AR145" s="14"/>
-      <c r="AS145" s="14"/>
+      <c r="AS145" s="14">
+        <v>14</v>
+      </c>
       <c r="AT145" s="14"/>
-      <c r="AU145" s="14"/>
+      <c r="AU145" s="14">
+        <v>3</v>
+      </c>
       <c r="AV145" s="14"/>
       <c r="AW145" s="14"/>
       <c r="AX145" s="14"/>
@@ -28803,27 +29009,27 @@
       <c r="AZ145" s="14"/>
       <c r="BA145" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="BB145" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null143</v>
+        <v>book</v>
       </c>
       <c r="BC145" s="13" t="str" cm="1">
         <f t="array" ref="BC145">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null143 = 143("null143", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000003))</v>
+        <v>val book = 143("book", { mirage }, 3, 30, 1.00, m(1.0, 5.0, 5.0, 10.0, 3.0, 2.0), a(1.0, 3.0, 0.0, 0.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 1.0, 0.0, 0.0, 0.0, 14.0, 0.0, 3.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xD6D6D6, 0x654B17, 0x654B17, 0x000000))</v>
       </c>
       <c r="BD145" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null143.name=null</v>
+        <v>mirageFairy2019.fairy.book.name=Bookia</v>
       </c>
       <c r="BE145" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null143.name=nullnull</v>
+        <v>mirageFairy2019.fairy.book.name=本精ボーキャ</v>
       </c>
       <c r="BF145" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
-        <v>0</v>
+        <v>1.9357622272015977</v>
       </c>
     </row>
     <row r="146" spans="1:58" x14ac:dyDescent="0.15">
@@ -28833,33 +29039,39 @@
       <c r="B146" s="4">
         <v>1</v>
       </c>
-      <c r="C146" s="4"/>
-      <c r="D146" s="4"/>
+      <c r="C146" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>400</v>
+      </c>
       <c r="E146" s="6" t="s">
-        <v>1054</v>
+        <v>223</v>
       </c>
       <c r="F146" s="6" t="s">
-        <v>1038</v>
+        <v>1053</v>
       </c>
       <c r="G146" s="6" t="s">
-        <v>1038</v>
+        <v>1069</v>
       </c>
       <c r="H146" s="6" t="s">
-        <v>1038</v>
+        <v>1076</v>
       </c>
       <c r="I146" s="6" t="s">
         <v>983</v>
       </c>
       <c r="J146" s="11" t="s">
-        <v>1061</v>
+        <v>1084</v>
       </c>
       <c r="K146" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L146" s="8">
-        <v>50</v>
-      </c>
-      <c r="M146" s="7"/>
+        <v>96</v>
+      </c>
+      <c r="M146" s="7">
+        <v>5</v>
+      </c>
       <c r="N146" s="7"/>
       <c r="O146" s="7"/>
       <c r="P146" s="7"/>
@@ -28867,28 +29079,28 @@
       <c r="R146" s="7">
         <v>10</v>
       </c>
-      <c r="S146" s="5">
-        <v>0.01</v>
+      <c r="S146" s="18">
+        <v>1</v>
       </c>
       <c r="T146" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>1.681792830507429</v>
       </c>
       <c r="U146" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M146:R146)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.93303299153680741</v>
       </c>
       <c r="V146" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.5691681957935013</v>
       </c>
       <c r="W146" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>150.64014679617611</v>
       </c>
       <c r="X146" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>50.213382265392042</v>
       </c>
       <c r="Y146" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -28908,7 +29120,7 @@
       </c>
       <c r="AC146" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
+        <v>100.42676453078408</v>
       </c>
       <c r="AD146" s="14"/>
       <c r="AE146" s="14"/>
@@ -28916,42 +29128,52 @@
       <c r="AG146" s="14"/>
       <c r="AH146" s="14"/>
       <c r="AI146" s="14"/>
-      <c r="AJ146" s="14"/>
+      <c r="AJ146" s="14">
+        <v>2</v>
+      </c>
       <c r="AK146" s="14"/>
       <c r="AL146" s="14"/>
       <c r="AM146" s="14"/>
       <c r="AN146" s="14"/>
-      <c r="AO146" s="14"/>
+      <c r="AO146" s="14">
+        <v>5</v>
+      </c>
       <c r="AP146" s="14"/>
-      <c r="AQ146" s="14"/>
+      <c r="AQ146" s="14">
+        <v>7</v>
+      </c>
       <c r="AR146" s="14"/>
       <c r="AS146" s="14"/>
       <c r="AT146" s="14"/>
-      <c r="AU146" s="14"/>
+      <c r="AU146" s="14">
+        <v>14</v>
+      </c>
       <c r="AV146" s="14"/>
       <c r="AW146" s="14"/>
       <c r="AX146" s="14"/>
-      <c r="AY146" s="14"/>
+      <c r="AY146" s="14">
+        <v>1</v>
+      </c>
       <c r="AZ146" s="14"/>
       <c r="BA146" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="BB146" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null144</v>
+        <v>bedrock</v>
       </c>
       <c r="BC146" s="13" t="str" cm="1">
         <f t="array" ref="BC146">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null144 = 144("null144", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000004))</v>
+        <v>val bedrock = 144("bedrock", { mirage }, 4, 96, 1.00, m(5.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 2.0, 0.0, 0.0, 0.0, 0.0, 5.0, 0.0, 7.0, 0.0, 0.0, 0.0, 14.0, 0.0, 0.0, 0.0, 1.0, 0.0), c(0x7C7C7C, 0xB4B4B4, 0x484848, 0x040404))</v>
       </c>
       <c r="BD146" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null144.name=null</v>
+        <v>mirageFairy2019.fairy.bedrock.name=Bedrockia</v>
       </c>
       <c r="BE146" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null144.name=nullnull</v>
+        <v>mirageFairy2019.fairy.bedrock.name=岩盤精ベドロッキャ</v>
       </c>
       <c r="BF146" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
@@ -28965,58 +29187,68 @@
       <c r="B147" s="4">
         <v>1</v>
       </c>
-      <c r="C147" s="4"/>
-      <c r="D147" s="4"/>
+      <c r="C147" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="D147" s="4" t="s">
+        <v>405</v>
+      </c>
       <c r="E147" s="6" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
       <c r="F147" s="6" t="s">
-        <v>1038</v>
+        <v>1057</v>
       </c>
       <c r="G147" s="6" t="s">
-        <v>1038</v>
+        <v>1072</v>
       </c>
       <c r="H147" s="6" t="s">
-        <v>1038</v>
+        <v>1079</v>
       </c>
       <c r="I147" s="6" t="s">
         <v>983</v>
       </c>
       <c r="J147" s="11" t="s">
-        <v>1062</v>
+        <v>1085</v>
       </c>
       <c r="K147" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L147" s="8">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="M147" s="7"/>
-      <c r="N147" s="7"/>
-      <c r="O147" s="7"/>
+      <c r="N147" s="7">
+        <v>1</v>
+      </c>
+      <c r="O147" s="7">
+        <v>8</v>
+      </c>
       <c r="P147" s="7"/>
-      <c r="Q147" s="7"/>
+      <c r="Q147" s="7">
+        <v>10</v>
+      </c>
       <c r="R147" s="7">
-        <v>10</v>
-      </c>
-      <c r="S147" s="5">
-        <v>0.01</v>
+        <v>1</v>
+      </c>
+      <c r="S147" s="18">
+        <v>1</v>
       </c>
       <c r="T147" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>1.681792830507429</v>
       </c>
       <c r="U147" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M147:R147)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.87055056329612412</v>
       </c>
       <c r="V147" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.4640856959456254</v>
       </c>
       <c r="W147" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>40.994399486477512</v>
       </c>
       <c r="X147" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -29024,11 +29256,11 @@
       </c>
       <c r="Y147" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>2.0497199743238754</v>
       </c>
       <c r="Z147" s="9">
         <f>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>16.397759794591003</v>
       </c>
       <c r="AA147" s="9">
         <f>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -29036,54 +29268,78 @@
       </c>
       <c r="AB147" s="9">
         <f>テーブル1[[#This Row],[基礎Aqua]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>20.497199743238756</v>
       </c>
       <c r="AC147" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
-      </c>
-      <c r="AD147" s="14"/>
+        <v>2.0497199743238754</v>
+      </c>
+      <c r="AD147" s="14">
+        <v>2</v>
+      </c>
       <c r="AE147" s="14"/>
-      <c r="AF147" s="14"/>
+      <c r="AF147" s="14">
+        <v>1</v>
+      </c>
       <c r="AG147" s="14"/>
       <c r="AH147" s="14"/>
-      <c r="AI147" s="14"/>
+      <c r="AI147" s="14">
+        <v>2</v>
+      </c>
       <c r="AJ147" s="14"/>
-      <c r="AK147" s="14"/>
+      <c r="AK147" s="14">
+        <v>8</v>
+      </c>
       <c r="AL147" s="14"/>
       <c r="AM147" s="14"/>
       <c r="AN147" s="14"/>
       <c r="AO147" s="14"/>
-      <c r="AP147" s="14"/>
-      <c r="AQ147" s="14"/>
-      <c r="AR147" s="14"/>
-      <c r="AS147" s="14"/>
-      <c r="AT147" s="14"/>
-      <c r="AU147" s="14"/>
+      <c r="AP147" s="14">
+        <v>1</v>
+      </c>
+      <c r="AQ147" s="14">
+        <v>1</v>
+      </c>
+      <c r="AR147" s="14">
+        <v>6</v>
+      </c>
+      <c r="AS147" s="14">
+        <v>4</v>
+      </c>
+      <c r="AT147" s="14">
+        <v>1</v>
+      </c>
+      <c r="AU147" s="14">
+        <v>4</v>
+      </c>
       <c r="AV147" s="14"/>
       <c r="AW147" s="14"/>
       <c r="AX147" s="14"/>
-      <c r="AY147" s="14"/>
-      <c r="AZ147" s="14"/>
+      <c r="AY147" s="14">
+        <v>10</v>
+      </c>
+      <c r="AZ147" s="14">
+        <v>10</v>
+      </c>
       <c r="BA147" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="BB147" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null145</v>
+        <v>bat</v>
       </c>
       <c r="BC147" s="13" t="str" cm="1">
         <f t="array" ref="BC147">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null145 = 145("null145", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000005))</v>
+        <v>val bat = 145("bat", { mirage }, 4, 28, 1.00, m(0.0, 1.0, 8.0, 0.0, 10.0, 1.0), a(2.0, 0.0, 1.0, 0.0, 0.0, 2.0, 0.0, 8.0, 0.0, 0.0, 0.0, 0.0, 1.0, 1.0, 6.0, 4.0, 1.0, 4.0, 0.0, 0.0, 0.0, 10.0, 10.0), c(0x4C3E30, 0x5B482B, 0x2C2014, 0x221F1D))</v>
       </c>
       <c r="BD147" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null145.name=null</v>
+        <v>mirageFairy2019.fairy.bat.name=Batia</v>
       </c>
       <c r="BE147" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null145.name=nullnull</v>
+        <v>mirageFairy2019.fairy.bat.name=蝙蝠精バーチャ</v>
       </c>
       <c r="BF147" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
@@ -29097,70 +29353,78 @@
       <c r="B148" s="4">
         <v>1</v>
       </c>
-      <c r="C148" s="4"/>
-      <c r="D148" s="4"/>
+      <c r="C148" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="D148" s="4" t="s">
+        <v>802</v>
+      </c>
       <c r="E148" s="6" t="s">
-        <v>1056</v>
+        <v>1060</v>
       </c>
       <c r="F148" s="6" t="s">
-        <v>1038</v>
+        <v>1059</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>1038</v>
+        <v>1073</v>
       </c>
       <c r="H148" s="6" t="s">
-        <v>1038</v>
+        <v>1080</v>
       </c>
       <c r="I148" s="6" t="s">
-        <v>983</v>
+        <v>525</v>
       </c>
       <c r="J148" s="11" t="s">
-        <v>1063</v>
+        <v>1089</v>
       </c>
       <c r="K148" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L148" s="8">
-        <v>50</v>
-      </c>
-      <c r="M148" s="7"/>
-      <c r="N148" s="7"/>
-      <c r="O148" s="7"/>
+        <v>44</v>
+      </c>
+      <c r="M148" s="7">
+        <v>1</v>
+      </c>
+      <c r="N148" s="7">
+        <v>22</v>
+      </c>
+      <c r="O148" s="7">
+        <v>10</v>
+      </c>
       <c r="P148" s="7"/>
       <c r="Q148" s="7"/>
-      <c r="R148" s="7">
-        <v>10</v>
-      </c>
-      <c r="S148" s="5">
-        <v>0.01</v>
+      <c r="R148" s="7"/>
+      <c r="S148" s="18">
+        <v>1</v>
       </c>
       <c r="T148" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U148" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M148:R148)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.93303299153680741</v>
       </c>
       <c r="V148" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.8660659830736148</v>
       </c>
       <c r="W148" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>82.106903255239047</v>
       </c>
       <c r="X148" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>2.4880879774314861</v>
       </c>
       <c r="Y148" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>54.737935503492693</v>
       </c>
       <c r="Z148" s="9">
         <f>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>24.880879774314863</v>
       </c>
       <c r="AA148" s="9">
         <f>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -29172,12 +29436,16 @@
       </c>
       <c r="AC148" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
-      </c>
-      <c r="AD148" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD148" s="14">
+        <v>6</v>
+      </c>
       <c r="AE148" s="14"/>
       <c r="AF148" s="14"/>
-      <c r="AG148" s="14"/>
+      <c r="AG148" s="14">
+        <v>3</v>
+      </c>
       <c r="AH148" s="14"/>
       <c r="AI148" s="14"/>
       <c r="AJ148" s="14"/>
@@ -29185,13 +29453,21 @@
       <c r="AL148" s="14"/>
       <c r="AM148" s="14"/>
       <c r="AN148" s="14"/>
-      <c r="AO148" s="14"/>
+      <c r="AO148" s="14">
+        <v>13</v>
+      </c>
       <c r="AP148" s="14"/>
-      <c r="AQ148" s="14"/>
+      <c r="AQ148" s="14">
+        <v>1</v>
+      </c>
       <c r="AR148" s="14"/>
-      <c r="AS148" s="14"/>
+      <c r="AS148" s="14">
+        <v>5</v>
+      </c>
       <c r="AT148" s="14"/>
-      <c r="AU148" s="14"/>
+      <c r="AU148" s="14">
+        <v>1</v>
+      </c>
       <c r="AV148" s="14"/>
       <c r="AW148" s="14"/>
       <c r="AX148" s="14"/>
@@ -29199,23 +29475,23 @@
       <c r="AZ148" s="14"/>
       <c r="BA148" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="BB148" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>null146</v>
+        <v>curseOfVanishing</v>
       </c>
       <c r="BC148" s="13" t="str" cm="1">
         <f t="array" ref="BC148">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val null146 = 146("null146", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000006))</v>
+        <v>val curseOfVanishing = 146("curse_of_vanishing", { enchant }, 5, 44, 1.00, m(1.0, 22.0, 10.0, 0.0, 0.0, 0.0), a(6.0, 0.0, 0.0, 3.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 13.0, 0.0, 1.0, 0.0, 5.0, 0.0, 1.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xD0C2FF, 0xFF003B, 0x370000, 0xE2BBFF))</v>
       </c>
       <c r="BD148" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.null146.name=null</v>
+        <v>mirageFairy2019.fairy.curse_of_vanishing.name=Curse Ofe Vanishingia</v>
       </c>
       <c r="BE148" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.null146.name=nullnull</v>
+        <v>mirageFairy2019.fairy.curse_of_vanishing.name=消滅呪精ツルセオフェヴァニシンギャ</v>
       </c>
       <c r="BF148" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
@@ -29229,70 +29505,78 @@
       <c r="B149" s="4">
         <v>1</v>
       </c>
-      <c r="C149" s="4"/>
-      <c r="D149" s="4"/>
+      <c r="C149" s="4" t="s">
+        <v>605</v>
+      </c>
+      <c r="D149" s="4" t="s">
+        <v>606</v>
+      </c>
       <c r="E149" s="6" t="s">
-        <v>1067</v>
+        <v>1051</v>
       </c>
       <c r="F149" s="6" t="s">
-        <v>1065</v>
+        <v>1052</v>
       </c>
       <c r="G149" s="6" t="s">
         <v>1068</v>
       </c>
       <c r="H149" s="6" t="s">
-        <v>1066</v>
+        <v>1075</v>
       </c>
       <c r="I149" s="6" t="s">
         <v>983</v>
       </c>
       <c r="J149" s="11" t="s">
-        <v>1064</v>
+        <v>1091</v>
       </c>
       <c r="K149" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L149" s="8">
-        <v>50</v>
-      </c>
-      <c r="M149" s="7"/>
-      <c r="N149" s="7"/>
-      <c r="O149" s="7"/>
+        <v>80</v>
+      </c>
+      <c r="M149" s="7">
+        <v>10</v>
+      </c>
+      <c r="N149" s="7">
+        <v>10</v>
+      </c>
+      <c r="O149" s="7">
+        <v>10</v>
+      </c>
       <c r="P149" s="7"/>
       <c r="Q149" s="7"/>
-      <c r="R149" s="7">
-        <v>10</v>
-      </c>
-      <c r="S149" s="5">
-        <v>0.01</v>
+      <c r="R149" s="7"/>
+      <c r="S149" s="18">
+        <v>1</v>
       </c>
       <c r="T149" s="5">
         <f>2^((テーブル1[[#This Row],[レア]]-1)/4)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U149" s="5">
         <f>0.5^(((テーブル1[[#This Row],[基礎Shine]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Fire]]/MAX(M149:R149)+テーブル1[[#This Row],[基礎Wind]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Gaia]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Aqua]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])+テーブル1[[#This Row],[基礎Dark]]/MAX(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]]))-1)/5)</f>
-        <v>1</v>
+        <v>0.75785828325519911</v>
       </c>
       <c r="V149" s="5">
         <f>テーブル1[[#This Row],[特殊倍率]]*テーブル1[[#This Row],[分散度倍率]]*テーブル1[[#This Row],[レア度倍率]]</f>
-        <v>0.01</v>
+        <v>1.5157165665103982</v>
       </c>
       <c r="W149" s="10">
         <f>テーブル1[[#This Row],[コスト]]*テーブル1[[#This Row],[効率]]</f>
-        <v>0.5</v>
+        <v>121.25732532083185</v>
       </c>
       <c r="X149" s="9">
         <f>テーブル1[[#This Row],[基礎Shine]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>40.419108440277277</v>
       </c>
       <c r="Y149" s="9">
         <f>テーブル1[[#This Row],[基礎Fire]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>40.419108440277277</v>
       </c>
       <c r="Z149" s="9">
         <f>テーブル1[[#This Row],[基礎Wind]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0</v>
+        <v>40.419108440277277</v>
       </c>
       <c r="AA149" s="9">
         <f>テーブル1[[#This Row],[基礎Gaia]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
@@ -29304,50 +29588,66 @@
       </c>
       <c r="AC149" s="9">
         <f>テーブル1[[#This Row],[基礎Dark]]*テーブル1[[#This Row],[合計値]]/SUM(テーブル1[[#This Row],[基礎Shine]:[基礎Dark]])</f>
-        <v>0.5</v>
-      </c>
-      <c r="AD149" s="14"/>
-      <c r="AE149" s="14"/>
+        <v>0</v>
+      </c>
+      <c r="AD149" s="14">
+        <v>5</v>
+      </c>
+      <c r="AE149" s="14">
+        <v>2</v>
+      </c>
       <c r="AF149" s="14"/>
       <c r="AG149" s="14"/>
       <c r="AH149" s="14"/>
       <c r="AI149" s="14"/>
       <c r="AJ149" s="14"/>
       <c r="AK149" s="14"/>
-      <c r="AL149" s="14"/>
+      <c r="AL149" s="14">
+        <v>23</v>
+      </c>
       <c r="AM149" s="14"/>
       <c r="AN149" s="14"/>
-      <c r="AO149" s="14"/>
-      <c r="AP149" s="14"/>
+      <c r="AO149" s="14">
+        <v>3</v>
+      </c>
+      <c r="AP149" s="14">
+        <v>1</v>
+      </c>
       <c r="AQ149" s="14"/>
       <c r="AR149" s="14"/>
-      <c r="AS149" s="14"/>
+      <c r="AS149" s="14">
+        <v>9</v>
+      </c>
       <c r="AT149" s="14"/>
-      <c r="AU149" s="14"/>
+      <c r="AU149" s="14">
+        <v>1</v>
+      </c>
       <c r="AV149" s="14"/>
       <c r="AW149" s="14"/>
       <c r="AX149" s="14"/>
-      <c r="AY149" s="14"/>
+      <c r="AY149" s="14">
+        <v>5</v>
+      </c>
       <c r="AZ149" s="14"/>
       <c r="BA149" s="13">
         <f>SUM(テーブル1[[#This Row],[攻撃]:[感覚]])</f>
-        <v>0</v>
+        <v>49</v>
       </c>
       <c r="BB149" s="13" t="str">
         <f>LOWER(LEFT(テーブル1[[#This Row],[Type]],1))&amp;MID(SUBSTITUTE(PROPER(テーブル1[[#This Row],[Type]]),"_",""),2,LEN(テーブル1[[#This Row],[Type]]))</f>
-        <v>ruby</v>
+        <v>gravity</v>
       </c>
       <c r="BC149" s="13" t="str" cm="1">
         <f t="array" ref="BC149">"val "&amp;テーブル1[[#This Row],[Camel Case]]&amp;" = "&amp;テーブル1[[#This Row],[No]]&amp;"("""&amp;テーブル1[[#This Row],[Type]]&amp;""", { "&amp;_xlfn.XLOOKUP(テーブル1[[#This Row],[上位妖精]], テーブル1[Type],テーブル1[Camel Case],"null")&amp;" }, "&amp;テーブル1[[#This Row],[レア]]&amp;", "&amp;テーブル1[[#This Row],[コスト]]&amp;", "&amp;TEXT(テーブル1[[#This Row],[特殊倍率]], "0.00")&amp;", m("&amp;TEXT(テーブル1[[#This Row],[基礎Shine]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Fire]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Wind]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Gaia]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Aqua]]*1, "0.0")&amp;", "&amp;TEXT(テーブル1[[#This Row],[基礎Dark]]*1, "0.0")&amp;"), a("&amp;_xlfn.TEXTJOIN(", ",FALSE,TEXT(テーブル1[[#This Row],[攻撃]:[感覚]]*1, "0.0"))&amp;"), c("&amp;テーブル1[[#This Row],[Color]]&amp;"))"</f>
-        <v>val ruby = 147("ruby", { mirage }, 1, 50, 0.01, m(0.0, 0.0, 0.0, 0.0, 0.0, 10.0), a(0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0), c(0xFF00FF, 0xFF00FF, 0x000000, 0x000007))</v>
+        <v>val gravity = 147("gravity", { mirage }, 5, 80, 1.00, m(10.0, 10.0, 10.0, 0.0, 0.0, 0.0), a(5.0, 2.0, 0.0, 0.0, 0.0, 0.0, 0.0, 0.0, 23.0, 0.0, 0.0, 3.0, 1.0, 0.0, 0.0, 9.0, 0.0, 1.0, 0.0, 0.0, 0.0, 5.0, 0.0), c(0xC2A7F2, 0x3600FF, 0x2A00B1, 0x110047))</v>
       </c>
       <c r="BD149" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[英名]]</f>
-        <v>mirageFairy2019.fairy.ruby.name=Rubia</v>
+        <v>mirageFairy2019.fairy.gravity.name=Gravitia</v>
       </c>
       <c r="BE149" s="13" t="str">
         <f>"mirageFairy2019.fairy."&amp;テーブル1[[#This Row],[Type]]&amp;".name="&amp;テーブル1[[#This Row],[短縮和名]]&amp;テーブル1[[#This Row],[和名]]</f>
-        <v>mirageFairy2019.fairy.ruby.name=紅玉精ルービャ</v>
+        <v>mirageFairy2019.fairy.gravity.name=重力精グラヴィーチャ</v>
       </c>
       <c r="BF149" s="13">
         <f>テーブル1[[#This Row],[Gaia]]*(テーブル1[[#This Row],[Aqua]]+テーブル1[[#This Row],[収穫]])*テーブル1[[#This Row],[効率]]/テーブル1[[#This Row],[コスト]]</f>
@@ -29405,7 +29705,7 @@
       <c r="R150" s="7">
         <v>82</v>
       </c>
-      <c r="S150" s="5">
+      <c r="S150" s="18">
         <v>1</v>
       </c>
       <c r="T150" s="5">
@@ -29573,7 +29873,7 @@
       <c r="R151" s="7">
         <v>41</v>
       </c>
-      <c r="S151" s="5">
+      <c r="S151" s="18">
         <v>1.2</v>
       </c>
       <c r="T151" s="5">
@@ -29723,7 +30023,7 @@
       <c r="P152" s="7"/>
       <c r="Q152" s="7"/>
       <c r="R152" s="7"/>
-      <c r="S152" s="5">
+      <c r="S152" s="18">
         <v>1</v>
       </c>
       <c r="T152" s="5" t="e">
@@ -29850,7 +30150,7 @@
         <v>10</v>
       </c>
       <c r="R153" s="7"/>
-      <c r="S153" s="5">
+      <c r="S153" s="18">
         <v>1</v>
       </c>
       <c r="T153" s="5" t="e">
@@ -29983,7 +30283,7 @@
         <v>8</v>
       </c>
       <c r="R154" s="7"/>
-      <c r="S154" s="5">
+      <c r="S154" s="18">
         <v>1</v>
       </c>
       <c r="T154" s="5" t="e">
@@ -30072,6 +30372,20 @@
         <v>#VALUE!</v>
       </c>
       <c r="BF154" s="13"/>
+    </row>
+    <row r="155" spans="1:58" x14ac:dyDescent="0.15">
+      <c r="E155" s="1" t="s">
+        <v>1067</v>
+      </c>
+      <c r="F155" s="1" t="s">
+        <v>1050</v>
+      </c>
+      <c r="G155" s="1" t="s">
+        <v>1065</v>
+      </c>
+      <c r="H155" s="1" t="s">
+        <v>1066</v>
+      </c>
     </row>
     <row r="156" spans="1:58" x14ac:dyDescent="0.15">
       <c r="BA156" s="16"/>

</xml_diff>